<commit_message>
made the ppd lab pretty
</commit_message>
<xml_diff>
--- a/Anul 3/Semestrul 1/PPD/labs/lab1/outC.xlsx
+++ b/Anul 3/Semestrul 1/PPD/labs/lab1/outC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\Github\University\Anul3\Semestrul1\PPD\labs\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\Github\University\Anul 3\Semestrul 1\PPD\labs\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DA422C30-81BB-41CD-B2BA-31A4666E6097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D0AA5B8A-254B-431D-AB07-2AC4DCC23317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outC" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,10 +546,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,11 +906,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -936,10 +936,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -950,8 +950,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
       <c r="C3">
         <v>4</v>
       </c>
@@ -960,8 +960,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4">
@@ -972,8 +972,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
       <c r="C5">
         <v>4</v>
       </c>
@@ -982,10 +982,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6">
@@ -996,8 +996,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7">
         <v>2</v>
       </c>
@@ -1006,8 +1006,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
       <c r="C8">
         <v>4</v>
       </c>
@@ -1016,8 +1016,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -1026,8 +1026,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
       <c r="C10">
         <v>16</v>
       </c>
@@ -1036,8 +1036,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11">
@@ -1048,8 +1048,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
       <c r="C12">
         <v>2</v>
       </c>
@@ -1058,8 +1058,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
       <c r="C13">
         <v>4</v>
       </c>
@@ -1068,8 +1068,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
       <c r="C14">
         <v>8</v>
       </c>
@@ -1078,8 +1078,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
       <c r="C15">
         <v>16</v>
       </c>
@@ -1088,10 +1088,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16">
@@ -1102,8 +1102,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
       <c r="C17">
         <v>2</v>
       </c>
@@ -1112,8 +1112,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
       <c r="C18">
         <v>4</v>
       </c>
@@ -1122,8 +1122,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
       <c r="C19">
         <v>8</v>
       </c>
@@ -1132,8 +1132,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
       <c r="C20">
         <v>16</v>
       </c>
@@ -1142,8 +1142,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21">
@@ -1154,8 +1154,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
       <c r="C22">
         <v>2</v>
       </c>
@@ -1164,8 +1164,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
       <c r="C23">
         <v>4</v>
       </c>
@@ -1174,8 +1174,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
       <c r="C24">
         <v>8</v>
       </c>
@@ -1184,8 +1184,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
       <c r="C25">
         <v>16</v>
       </c>
@@ -1194,10 +1194,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C26">
@@ -1208,8 +1208,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
       <c r="C27">
         <v>2</v>
       </c>
@@ -1218,8 +1218,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
       <c r="C28">
         <v>4</v>
       </c>
@@ -1228,8 +1228,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
       <c r="C29">
         <v>8</v>
       </c>
@@ -1238,8 +1238,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
       <c r="C30">
         <v>16</v>
       </c>
@@ -1248,8 +1248,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31">
@@ -1260,8 +1260,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="1"/>
       <c r="C32">
         <v>2</v>
       </c>
@@ -1270,8 +1270,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
       <c r="C33">
         <v>4</v>
       </c>
@@ -1280,8 +1280,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="1"/>
       <c r="C34">
         <v>8</v>
       </c>
@@ -1290,8 +1290,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="1"/>
       <c r="C35">
         <v>16</v>
       </c>
@@ -1301,18 +1301,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A6:A15"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="B21:B25"/>
     <mergeCell ref="B26:B30"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="A26:A35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="A6:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>